<commit_message>
Update incoming inspection log templates
</commit_message>
<xml_diff>
--- a/dist/modules/templates/Incoming Inspection Log Template.xlsx
+++ b/dist/modules/templates/Incoming Inspection Log Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\Pragmatic\Projects\DBA-Automation-Tools\dist\modules\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB43548-58A1-43F6-98CB-C44A1EC55EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943FAFD-CA6A-4C6C-985F-55231CCD1B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="1380" windowWidth="19380" windowHeight="12045" xr2:uid="{787A15B7-D0B2-4895-82D1-FA4613D51671}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Revision History" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incoming Log 2020'!$A$2:$K$75</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Incoming Log 2020'!$A$1:$K$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incoming Log 2020'!$A$2:$J$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Incoming Log 2020'!$A$1:$J$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Incoming Inspection Log</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Inspection Number</t>
-  </si>
-  <si>
-    <t>Receiver ID</t>
   </si>
 </sst>
 </file>
@@ -684,6 +681,12 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -693,11 +696,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -705,12 +703,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1029,11 +1026,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC75"/>
+  <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,26 +1038,25 @@
     <col min="1" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="24" width="11.7109375" customWidth="1"/>
+    <col min="5" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="23" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="40"/>
+    </row>
+    <row r="2" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1085,15 +1081,13 @@
       <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="51" t="s">
+      <c r="I2" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="J2" s="37" t="s">
         <v>10</v>
       </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1107,9 +1101,8 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
@@ -1119,13 +1112,12 @@
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
       <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="22"/>
-      <c r="AC3" t="s">
+      <c r="J3" s="22"/>
+      <c r="AB3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="23"/>
       <c r="C4" s="24"/>
@@ -1135,13 +1127,12 @@
       <c r="G4" s="24"/>
       <c r="H4" s="25"/>
       <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="26"/>
-      <c r="AC4" t="s">
+      <c r="J4" s="26"/>
+      <c r="AB4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
@@ -1151,10 +1142,9 @@
       <c r="G5" s="24"/>
       <c r="H5" s="25"/>
       <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="26"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="23"/>
       <c r="C6" s="24"/>
@@ -1164,10 +1154,9 @@
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
       <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="26"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
@@ -1177,13 +1166,12 @@
       <c r="G7" s="24"/>
       <c r="H7" s="25"/>
       <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="26"/>
-      <c r="AC7" t="s">
+      <c r="J7" s="26"/>
+      <c r="AB7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24"/>
@@ -1193,13 +1181,12 @@
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
       <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="26"/>
-      <c r="AC8" t="s">
+      <c r="J8" s="26"/>
+      <c r="AB8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
@@ -1209,10 +1196,9 @@
       <c r="G9" s="24"/>
       <c r="H9" s="25"/>
       <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="26"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
@@ -1222,10 +1208,9 @@
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
       <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="26"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
@@ -1235,10 +1220,9 @@
       <c r="G11" s="24"/>
       <c r="H11" s="25"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="26"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
@@ -1248,10 +1232,9 @@
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
       <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="26"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
@@ -1261,10 +1244,9 @@
       <c r="G13" s="24"/>
       <c r="H13" s="25"/>
       <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="26"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -1274,10 +1256,9 @@
       <c r="G14" s="24"/>
       <c r="H14" s="25"/>
       <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="26"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
@@ -1287,10 +1268,9 @@
       <c r="G15" s="24"/>
       <c r="H15" s="25"/>
       <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="26"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
@@ -1300,10 +1280,9 @@
       <c r="G16" s="24"/>
       <c r="H16" s="25"/>
       <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="26"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24"/>
@@ -1313,10 +1292,9 @@
       <c r="G17" s="24"/>
       <c r="H17" s="25"/>
       <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="26"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24"/>
@@ -1326,10 +1304,9 @@
       <c r="G18" s="24"/>
       <c r="H18" s="25"/>
       <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="26"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
@@ -1339,10 +1316,9 @@
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
       <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="26"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24"/>
@@ -1352,10 +1328,9 @@
       <c r="G20" s="24"/>
       <c r="H20" s="25"/>
       <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="26"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
@@ -1365,10 +1340,9 @@
       <c r="G21" s="24"/>
       <c r="H21" s="25"/>
       <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="26"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24"/>
@@ -1378,10 +1352,9 @@
       <c r="G22" s="24"/>
       <c r="H22" s="25"/>
       <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="26"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="23"/>
       <c r="C23" s="24"/>
@@ -1391,10 +1364,9 @@
       <c r="G23" s="24"/>
       <c r="H23" s="25"/>
       <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="26"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
@@ -1404,10 +1376,9 @@
       <c r="G24" s="24"/>
       <c r="H24" s="25"/>
       <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="26"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="23"/>
       <c r="C25" s="24"/>
@@ -1417,10 +1388,9 @@
       <c r="G25" s="24"/>
       <c r="H25" s="25"/>
       <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="26"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="23"/>
       <c r="C26" s="24"/>
@@ -1430,10 +1400,9 @@
       <c r="G26" s="24"/>
       <c r="H26" s="25"/>
       <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="26"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="23"/>
       <c r="C27" s="24"/>
@@ -1443,10 +1412,9 @@
       <c r="G27" s="24"/>
       <c r="H27" s="25"/>
       <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="26"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="26"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="23"/>
       <c r="C28" s="30"/>
@@ -1456,10 +1424,9 @@
       <c r="G28" s="24"/>
       <c r="H28" s="25"/>
       <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="26"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="23"/>
       <c r="C29" s="24"/>
@@ -1469,10 +1436,9 @@
       <c r="G29" s="24"/>
       <c r="H29" s="25"/>
       <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="26"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="23"/>
       <c r="C30" s="24"/>
@@ -1482,10 +1448,9 @@
       <c r="G30" s="24"/>
       <c r="H30" s="25"/>
       <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="26"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="27"/>
       <c r="C31" s="24"/>
@@ -1495,10 +1460,9 @@
       <c r="G31" s="24"/>
       <c r="H31" s="25"/>
       <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="26"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="23"/>
       <c r="C32" s="24"/>
@@ -1508,10 +1472,9 @@
       <c r="G32" s="24"/>
       <c r="H32" s="25"/>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="26"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="26"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="23"/>
       <c r="C33" s="30"/>
@@ -1521,10 +1484,9 @@
       <c r="G33" s="24"/>
       <c r="H33" s="25"/>
       <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="26"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="26"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="23"/>
       <c r="C34" s="30"/>
@@ -1534,10 +1496,9 @@
       <c r="G34" s="24"/>
       <c r="H34" s="25"/>
       <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="26"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="26"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="23"/>
       <c r="C35" s="24"/>
@@ -1547,10 +1508,9 @@
       <c r="G35" s="24"/>
       <c r="H35" s="25"/>
       <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="26"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J35" s="26"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="23"/>
       <c r="C36" s="24"/>
@@ -1560,10 +1520,9 @@
       <c r="G36" s="24"/>
       <c r="H36" s="25"/>
       <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="26"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J36" s="26"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
@@ -1573,10 +1532,9 @@
       <c r="G37" s="24"/>
       <c r="H37" s="25"/>
       <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="26"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J37" s="26"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="23"/>
       <c r="C38" s="24"/>
@@ -1586,10 +1544,9 @@
       <c r="G38" s="24"/>
       <c r="H38" s="25"/>
       <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="26"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J38" s="26"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="23"/>
       <c r="C39" s="24"/>
@@ -1599,10 +1556,9 @@
       <c r="G39" s="24"/>
       <c r="H39" s="25"/>
       <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="26"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="26"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="23"/>
       <c r="C40" s="24"/>
@@ -1612,10 +1568,9 @@
       <c r="G40" s="24"/>
       <c r="H40" s="25"/>
       <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="26"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="26"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="23"/>
       <c r="C41" s="24"/>
@@ -1625,10 +1580,9 @@
       <c r="G41" s="24"/>
       <c r="H41" s="25"/>
       <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="26"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J41" s="26"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="23"/>
       <c r="C42" s="30"/>
@@ -1638,10 +1592,9 @@
       <c r="G42" s="24"/>
       <c r="H42" s="25"/>
       <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="26"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J42" s="26"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="23"/>
       <c r="C43" s="24"/>
@@ -1651,10 +1604,9 @@
       <c r="G43" s="24"/>
       <c r="H43" s="25"/>
       <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="26"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J43" s="26"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="23"/>
       <c r="C44" s="24"/>
@@ -1664,10 +1616,9 @@
       <c r="G44" s="24"/>
       <c r="H44" s="25"/>
       <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="26"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J44" s="26"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="23"/>
       <c r="C45" s="24"/>
@@ -1677,10 +1628,9 @@
       <c r="G45" s="24"/>
       <c r="H45" s="25"/>
       <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="26"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J45" s="26"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="23"/>
       <c r="C46" s="24"/>
@@ -1690,10 +1640,9 @@
       <c r="G46" s="24"/>
       <c r="H46" s="25"/>
       <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="26"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J46" s="26"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="23"/>
       <c r="C47" s="24"/>
@@ -1703,10 +1652,9 @@
       <c r="G47" s="24"/>
       <c r="H47" s="25"/>
       <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="26"/>
-    </row>
-    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="26"/>
+    </row>
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="23"/>
       <c r="C48" s="30"/>
@@ -1716,10 +1664,9 @@
       <c r="G48" s="24"/>
       <c r="H48" s="25"/>
       <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="26"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J48" s="26"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="23"/>
       <c r="C49" s="24"/>
@@ -1729,10 +1676,9 @@
       <c r="G49" s="24"/>
       <c r="H49" s="25"/>
       <c r="I49" s="29"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="26"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J49" s="26"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="23"/>
       <c r="C50" s="30"/>
@@ -1742,10 +1688,9 @@
       <c r="G50" s="24"/>
       <c r="H50" s="25"/>
       <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="26"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J50" s="26"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="23"/>
       <c r="C51" s="24"/>
@@ -1755,10 +1700,9 @@
       <c r="G51" s="24"/>
       <c r="H51" s="25"/>
       <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
-      <c r="K51" s="26"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J51" s="26"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="23"/>
       <c r="C52" s="24"/>
@@ -1768,10 +1712,9 @@
       <c r="G52" s="24"/>
       <c r="H52" s="25"/>
       <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
-      <c r="K52" s="26"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J52" s="26"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="23"/>
       <c r="C53" s="24"/>
@@ -1781,10 +1724,9 @@
       <c r="G53" s="24"/>
       <c r="H53" s="25"/>
       <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="26"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J53" s="26"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="23"/>
       <c r="C54" s="24"/>
@@ -1794,10 +1736,9 @@
       <c r="G54" s="24"/>
       <c r="H54" s="25"/>
       <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="26"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J54" s="26"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="23"/>
       <c r="C55" s="24"/>
@@ -1807,10 +1748,9 @@
       <c r="G55" s="24"/>
       <c r="H55" s="25"/>
       <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="26"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J55" s="26"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="23"/>
       <c r="C56" s="24"/>
@@ -1820,10 +1760,9 @@
       <c r="G56" s="24"/>
       <c r="H56" s="25"/>
       <c r="I56" s="29"/>
-      <c r="J56" s="29"/>
-      <c r="K56" s="26"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J56" s="26"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="23"/>
       <c r="C57" s="24"/>
@@ -1833,10 +1772,9 @@
       <c r="G57" s="24"/>
       <c r="H57" s="25"/>
       <c r="I57" s="29"/>
-      <c r="J57" s="29"/>
-      <c r="K57" s="26"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J57" s="26"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="23"/>
       <c r="C58" s="24"/>
@@ -1846,10 +1784,9 @@
       <c r="G58" s="24"/>
       <c r="H58" s="25"/>
       <c r="I58" s="29"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="26"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J58" s="26"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="23"/>
       <c r="C59" s="24"/>
@@ -1859,10 +1796,9 @@
       <c r="G59" s="24"/>
       <c r="H59" s="25"/>
       <c r="I59" s="29"/>
-      <c r="J59" s="29"/>
-      <c r="K59" s="26"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J59" s="26"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="23"/>
       <c r="C60" s="24"/>
@@ -1872,10 +1808,9 @@
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
       <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="26"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J60" s="26"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="23"/>
       <c r="C61" s="24"/>
@@ -1885,10 +1820,9 @@
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
       <c r="I61" s="29"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="26"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J61" s="26"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="23"/>
       <c r="C62" s="24"/>
@@ -1898,10 +1832,9 @@
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
       <c r="I62" s="29"/>
-      <c r="J62" s="29"/>
-      <c r="K62" s="26"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J62" s="26"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="23"/>
       <c r="C63" s="24"/>
@@ -1911,10 +1844,9 @@
       <c r="G63" s="24"/>
       <c r="H63" s="25"/>
       <c r="I63" s="29"/>
-      <c r="J63" s="29"/>
-      <c r="K63" s="26"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J63" s="26"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="23"/>
       <c r="C64" s="24"/>
@@ -1924,10 +1856,9 @@
       <c r="G64" s="24"/>
       <c r="H64" s="25"/>
       <c r="I64" s="29"/>
-      <c r="J64" s="29"/>
-      <c r="K64" s="26"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J64" s="26"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="23"/>
       <c r="C65" s="24"/>
@@ -1937,10 +1868,9 @@
       <c r="G65" s="24"/>
       <c r="H65" s="25"/>
       <c r="I65" s="29"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="26"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J65" s="26"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="23"/>
       <c r="C66" s="24"/>
@@ -1950,10 +1880,9 @@
       <c r="G66" s="24"/>
       <c r="H66" s="25"/>
       <c r="I66" s="29"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="26"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J66" s="26"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="23"/>
       <c r="C67" s="24"/>
@@ -1963,10 +1892,9 @@
       <c r="G67" s="24"/>
       <c r="H67" s="25"/>
       <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="26"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J67" s="26"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="23"/>
       <c r="C68" s="24"/>
@@ -1976,10 +1904,9 @@
       <c r="G68" s="24"/>
       <c r="H68" s="25"/>
       <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="26"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J68" s="26"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="23"/>
       <c r="C69" s="24"/>
@@ -1989,10 +1916,9 @@
       <c r="G69" s="24"/>
       <c r="H69" s="25"/>
       <c r="I69" s="29"/>
-      <c r="J69" s="29"/>
-      <c r="K69" s="26"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J69" s="26"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="23"/>
       <c r="C70" s="24"/>
@@ -2002,10 +1928,9 @@
       <c r="G70" s="24"/>
       <c r="H70" s="25"/>
       <c r="I70" s="29"/>
-      <c r="J70" s="29"/>
-      <c r="K70" s="26"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J70" s="26"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="23"/>
       <c r="C71" s="24"/>
@@ -2015,10 +1940,9 @@
       <c r="G71" s="24"/>
       <c r="H71" s="25"/>
       <c r="I71" s="29"/>
-      <c r="J71" s="29"/>
-      <c r="K71" s="26"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J71" s="26"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="23"/>
       <c r="C72" s="30"/>
@@ -2028,10 +1952,9 @@
       <c r="G72" s="24"/>
       <c r="H72" s="25"/>
       <c r="I72" s="29"/>
-      <c r="J72" s="29"/>
-      <c r="K72" s="26"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J72" s="26"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="23"/>
       <c r="C73" s="24"/>
@@ -2041,10 +1964,9 @@
       <c r="G73" s="24"/>
       <c r="H73" s="25"/>
       <c r="I73" s="29"/>
-      <c r="J73" s="29"/>
-      <c r="K73" s="26"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J73" s="26"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="23"/>
       <c r="C74" s="24"/>
@@ -2054,10 +1976,9 @@
       <c r="G74" s="24"/>
       <c r="H74" s="25"/>
       <c r="I74" s="29"/>
-      <c r="J74" s="29"/>
-      <c r="K74" s="26"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J74" s="26"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="23"/>
       <c r="C75" s="24"/>
@@ -2067,21 +1988,20 @@
       <c r="G75" s="24"/>
       <c r="H75" s="25"/>
       <c r="I75" s="29"/>
-      <c r="J75" s="29"/>
-      <c r="K75" s="26"/>
+      <c r="J75" s="26"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <autoFilter ref="A2:K75" xr:uid="{52620AD0-D81A-4707-BF25-930520122703}"/>
+  <autoFilter ref="A2:J75" xr:uid="{52620AD0-D81A-4707-BF25-930520122703}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J75" xr:uid="{95136ACE-3B61-4F2E-BC2F-785DA5FB4AA4}">
-      <formula1>$AC$7:$AC$8</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I75" xr:uid="{95136ACE-3B61-4F2E-BC2F-785DA5FB4AA4}">
+      <formula1>$AB$7:$AB$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I75" xr:uid="{A8A29524-CB88-4A40-9BD1-F8E9BD2459CB}">
-      <formula1>$AC$3:$AC$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H75" xr:uid="{A8A29524-CB88-4A40-9BD1-F8E9BD2459CB}">
+      <formula1>$AB$3:$AB$4</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -2123,16 +2043,16 @@
       <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42" t="s">
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
@@ -2144,60 +2064,60 @@
       <c r="C2" s="14">
         <v>44130</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="45" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="47"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="12"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="47"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="44"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="12"/>
       <c r="C4" s="15"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="47"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="12"/>
       <c r="C5" s="15"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="47"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="13"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="50"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2215,18 +2135,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update incoming inspection log
</commit_message>
<xml_diff>
--- a/dist/modules/templates/Incoming Inspection Log Template.xlsx
+++ b/dist/modules/templates/Incoming Inspection Log Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\Pragmatic\Projects\DBA-Automation-Tools\dist\modules\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943FAFD-CA6A-4C6C-985F-55231CCD1B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB43548-58A1-43F6-98CB-C44A1EC55EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="1380" windowWidth="19380" windowHeight="12045" xr2:uid="{787A15B7-D0B2-4895-82D1-FA4613D51671}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Revision History" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incoming Log 2020'!$A$2:$J$75</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Incoming Log 2020'!$A$1:$J$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incoming Log 2020'!$A$2:$K$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Incoming Log 2020'!$A$1:$K$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Incoming Inspection Log</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Inspection Number</t>
+  </si>
+  <si>
+    <t>Receiver ID</t>
   </si>
 </sst>
 </file>
@@ -681,12 +684,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -696,6 +693,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -703,11 +705,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1026,11 +1029,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB75"/>
+  <dimension ref="A1:AC75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I1:I1048576"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,25 +1041,26 @@
     <col min="1" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="23" width="11.7109375" customWidth="1"/>
+    <col min="5" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="24" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40"/>
-    </row>
-    <row r="2" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
+    </row>
+    <row r="2" spans="1:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1081,13 +1085,15 @@
       <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="K2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1101,8 +1107,9 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y2" s="1"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
@@ -1112,12 +1119,13 @@
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
       <c r="I3" s="28"/>
-      <c r="J3" s="22"/>
-      <c r="AB3" t="s">
+      <c r="J3" s="28"/>
+      <c r="K3" s="22"/>
+      <c r="AC3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="23"/>
       <c r="C4" s="24"/>
@@ -1127,12 +1135,13 @@
       <c r="G4" s="24"/>
       <c r="H4" s="25"/>
       <c r="I4" s="29"/>
-      <c r="J4" s="26"/>
-      <c r="AB4" t="s">
+      <c r="J4" s="29"/>
+      <c r="K4" s="26"/>
+      <c r="AC4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
@@ -1142,9 +1151,10 @@
       <c r="G5" s="24"/>
       <c r="H5" s="25"/>
       <c r="I5" s="29"/>
-      <c r="J5" s="26"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J5" s="29"/>
+      <c r="K5" s="26"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="23"/>
       <c r="C6" s="24"/>
@@ -1154,9 +1164,10 @@
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
       <c r="I6" s="29"/>
-      <c r="J6" s="26"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J6" s="29"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
@@ -1166,12 +1177,13 @@
       <c r="G7" s="24"/>
       <c r="H7" s="25"/>
       <c r="I7" s="29"/>
-      <c r="J7" s="26"/>
-      <c r="AB7" t="s">
+      <c r="J7" s="29"/>
+      <c r="K7" s="26"/>
+      <c r="AC7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24"/>
@@ -1181,12 +1193,13 @@
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
       <c r="I8" s="29"/>
-      <c r="J8" s="26"/>
-      <c r="AB8" t="s">
+      <c r="J8" s="29"/>
+      <c r="K8" s="26"/>
+      <c r="AC8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
@@ -1196,9 +1209,10 @@
       <c r="G9" s="24"/>
       <c r="H9" s="25"/>
       <c r="I9" s="29"/>
-      <c r="J9" s="26"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J9" s="29"/>
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
@@ -1208,9 +1222,10 @@
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
       <c r="I10" s="29"/>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J10" s="29"/>
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
@@ -1220,9 +1235,10 @@
       <c r="G11" s="24"/>
       <c r="H11" s="25"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="26"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J11" s="29"/>
+      <c r="K11" s="26"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
@@ -1232,9 +1248,10 @@
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
       <c r="I12" s="29"/>
-      <c r="J12" s="26"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J12" s="29"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
@@ -1244,9 +1261,10 @@
       <c r="G13" s="24"/>
       <c r="H13" s="25"/>
       <c r="I13" s="29"/>
-      <c r="J13" s="26"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J13" s="29"/>
+      <c r="K13" s="26"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -1256,9 +1274,10 @@
       <c r="G14" s="24"/>
       <c r="H14" s="25"/>
       <c r="I14" s="29"/>
-      <c r="J14" s="26"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J14" s="29"/>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
@@ -1268,9 +1287,10 @@
       <c r="G15" s="24"/>
       <c r="H15" s="25"/>
       <c r="I15" s="29"/>
-      <c r="J15" s="26"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J15" s="29"/>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
@@ -1280,9 +1300,10 @@
       <c r="G16" s="24"/>
       <c r="H16" s="25"/>
       <c r="I16" s="29"/>
-      <c r="J16" s="26"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="29"/>
+      <c r="K16" s="26"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24"/>
@@ -1292,9 +1313,10 @@
       <c r="G17" s="24"/>
       <c r="H17" s="25"/>
       <c r="I17" s="29"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="29"/>
+      <c r="K17" s="26"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24"/>
@@ -1304,9 +1326,10 @@
       <c r="G18" s="24"/>
       <c r="H18" s="25"/>
       <c r="I18" s="29"/>
-      <c r="J18" s="26"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="29"/>
+      <c r="K18" s="26"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
@@ -1316,9 +1339,10 @@
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
       <c r="I19" s="29"/>
-      <c r="J19" s="26"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="29"/>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24"/>
@@ -1328,9 +1352,10 @@
       <c r="G20" s="24"/>
       <c r="H20" s="25"/>
       <c r="I20" s="29"/>
-      <c r="J20" s="26"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="29"/>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
@@ -1340,9 +1365,10 @@
       <c r="G21" s="24"/>
       <c r="H21" s="25"/>
       <c r="I21" s="29"/>
-      <c r="J21" s="26"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="29"/>
+      <c r="K21" s="26"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24"/>
@@ -1352,9 +1378,10 @@
       <c r="G22" s="24"/>
       <c r="H22" s="25"/>
       <c r="I22" s="29"/>
-      <c r="J22" s="26"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="29"/>
+      <c r="K22" s="26"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="23"/>
       <c r="C23" s="24"/>
@@ -1364,9 +1391,10 @@
       <c r="G23" s="24"/>
       <c r="H23" s="25"/>
       <c r="I23" s="29"/>
-      <c r="J23" s="26"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="29"/>
+      <c r="K23" s="26"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
@@ -1376,9 +1404,10 @@
       <c r="G24" s="24"/>
       <c r="H24" s="25"/>
       <c r="I24" s="29"/>
-      <c r="J24" s="26"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="29"/>
+      <c r="K24" s="26"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="23"/>
       <c r="C25" s="24"/>
@@ -1388,9 +1417,10 @@
       <c r="G25" s="24"/>
       <c r="H25" s="25"/>
       <c r="I25" s="29"/>
-      <c r="J25" s="26"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="29"/>
+      <c r="K25" s="26"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="23"/>
       <c r="C26" s="24"/>
@@ -1400,9 +1430,10 @@
       <c r="G26" s="24"/>
       <c r="H26" s="25"/>
       <c r="I26" s="29"/>
-      <c r="J26" s="26"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="29"/>
+      <c r="K26" s="26"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="23"/>
       <c r="C27" s="24"/>
@@ -1412,9 +1443,10 @@
       <c r="G27" s="24"/>
       <c r="H27" s="25"/>
       <c r="I27" s="29"/>
-      <c r="J27" s="26"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="29"/>
+      <c r="K27" s="26"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="23"/>
       <c r="C28" s="30"/>
@@ -1424,9 +1456,10 @@
       <c r="G28" s="24"/>
       <c r="H28" s="25"/>
       <c r="I28" s="29"/>
-      <c r="J28" s="26"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="29"/>
+      <c r="K28" s="26"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="23"/>
       <c r="C29" s="24"/>
@@ -1436,9 +1469,10 @@
       <c r="G29" s="24"/>
       <c r="H29" s="25"/>
       <c r="I29" s="29"/>
-      <c r="J29" s="26"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="29"/>
+      <c r="K29" s="26"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="23"/>
       <c r="C30" s="24"/>
@@ -1448,9 +1482,10 @@
       <c r="G30" s="24"/>
       <c r="H30" s="25"/>
       <c r="I30" s="29"/>
-      <c r="J30" s="26"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="29"/>
+      <c r="K30" s="26"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="27"/>
       <c r="C31" s="24"/>
@@ -1460,9 +1495,10 @@
       <c r="G31" s="24"/>
       <c r="H31" s="25"/>
       <c r="I31" s="29"/>
-      <c r="J31" s="26"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="29"/>
+      <c r="K31" s="26"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="23"/>
       <c r="C32" s="24"/>
@@ -1472,9 +1508,10 @@
       <c r="G32" s="24"/>
       <c r="H32" s="25"/>
       <c r="I32" s="29"/>
-      <c r="J32" s="26"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="29"/>
+      <c r="K32" s="26"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="23"/>
       <c r="C33" s="30"/>
@@ -1484,9 +1521,10 @@
       <c r="G33" s="24"/>
       <c r="H33" s="25"/>
       <c r="I33" s="29"/>
-      <c r="J33" s="26"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="29"/>
+      <c r="K33" s="26"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="23"/>
       <c r="C34" s="30"/>
@@ -1496,9 +1534,10 @@
       <c r="G34" s="24"/>
       <c r="H34" s="25"/>
       <c r="I34" s="29"/>
-      <c r="J34" s="26"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="29"/>
+      <c r="K34" s="26"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="23"/>
       <c r="C35" s="24"/>
@@ -1508,9 +1547,10 @@
       <c r="G35" s="24"/>
       <c r="H35" s="25"/>
       <c r="I35" s="29"/>
-      <c r="J35" s="26"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="29"/>
+      <c r="K35" s="26"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="23"/>
       <c r="C36" s="24"/>
@@ -1520,9 +1560,10 @@
       <c r="G36" s="24"/>
       <c r="H36" s="25"/>
       <c r="I36" s="29"/>
-      <c r="J36" s="26"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="29"/>
+      <c r="K36" s="26"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
@@ -1532,9 +1573,10 @@
       <c r="G37" s="24"/>
       <c r="H37" s="25"/>
       <c r="I37" s="29"/>
-      <c r="J37" s="26"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="29"/>
+      <c r="K37" s="26"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="23"/>
       <c r="C38" s="24"/>
@@ -1544,9 +1586,10 @@
       <c r="G38" s="24"/>
       <c r="H38" s="25"/>
       <c r="I38" s="29"/>
-      <c r="J38" s="26"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="29"/>
+      <c r="K38" s="26"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="23"/>
       <c r="C39" s="24"/>
@@ -1556,9 +1599,10 @@
       <c r="G39" s="24"/>
       <c r="H39" s="25"/>
       <c r="I39" s="29"/>
-      <c r="J39" s="26"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="29"/>
+      <c r="K39" s="26"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="23"/>
       <c r="C40" s="24"/>
@@ -1568,9 +1612,10 @@
       <c r="G40" s="24"/>
       <c r="H40" s="25"/>
       <c r="I40" s="29"/>
-      <c r="J40" s="26"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="29"/>
+      <c r="K40" s="26"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="23"/>
       <c r="C41" s="24"/>
@@ -1580,9 +1625,10 @@
       <c r="G41" s="24"/>
       <c r="H41" s="25"/>
       <c r="I41" s="29"/>
-      <c r="J41" s="26"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="29"/>
+      <c r="K41" s="26"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="23"/>
       <c r="C42" s="30"/>
@@ -1592,9 +1638,10 @@
       <c r="G42" s="24"/>
       <c r="H42" s="25"/>
       <c r="I42" s="29"/>
-      <c r="J42" s="26"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J42" s="29"/>
+      <c r="K42" s="26"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="23"/>
       <c r="C43" s="24"/>
@@ -1604,9 +1651,10 @@
       <c r="G43" s="24"/>
       <c r="H43" s="25"/>
       <c r="I43" s="29"/>
-      <c r="J43" s="26"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="29"/>
+      <c r="K43" s="26"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="23"/>
       <c r="C44" s="24"/>
@@ -1616,9 +1664,10 @@
       <c r="G44" s="24"/>
       <c r="H44" s="25"/>
       <c r="I44" s="29"/>
-      <c r="J44" s="26"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="29"/>
+      <c r="K44" s="26"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="23"/>
       <c r="C45" s="24"/>
@@ -1628,9 +1677,10 @@
       <c r="G45" s="24"/>
       <c r="H45" s="25"/>
       <c r="I45" s="29"/>
-      <c r="J45" s="26"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="29"/>
+      <c r="K45" s="26"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="23"/>
       <c r="C46" s="24"/>
@@ -1640,9 +1690,10 @@
       <c r="G46" s="24"/>
       <c r="H46" s="25"/>
       <c r="I46" s="29"/>
-      <c r="J46" s="26"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J46" s="29"/>
+      <c r="K46" s="26"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="23"/>
       <c r="C47" s="24"/>
@@ -1652,9 +1703,10 @@
       <c r="G47" s="24"/>
       <c r="H47" s="25"/>
       <c r="I47" s="29"/>
-      <c r="J47" s="26"/>
-    </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="29"/>
+      <c r="K47" s="26"/>
+    </row>
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="23"/>
       <c r="C48" s="30"/>
@@ -1664,9 +1716,10 @@
       <c r="G48" s="24"/>
       <c r="H48" s="25"/>
       <c r="I48" s="29"/>
-      <c r="J48" s="26"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J48" s="29"/>
+      <c r="K48" s="26"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="23"/>
       <c r="C49" s="24"/>
@@ -1676,9 +1729,10 @@
       <c r="G49" s="24"/>
       <c r="H49" s="25"/>
       <c r="I49" s="29"/>
-      <c r="J49" s="26"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J49" s="29"/>
+      <c r="K49" s="26"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="23"/>
       <c r="C50" s="30"/>
@@ -1688,9 +1742,10 @@
       <c r="G50" s="24"/>
       <c r="H50" s="25"/>
       <c r="I50" s="29"/>
-      <c r="J50" s="26"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J50" s="29"/>
+      <c r="K50" s="26"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="23"/>
       <c r="C51" s="24"/>
@@ -1700,9 +1755,10 @@
       <c r="G51" s="24"/>
       <c r="H51" s="25"/>
       <c r="I51" s="29"/>
-      <c r="J51" s="26"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J51" s="29"/>
+      <c r="K51" s="26"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="23"/>
       <c r="C52" s="24"/>
@@ -1712,9 +1768,10 @@
       <c r="G52" s="24"/>
       <c r="H52" s="25"/>
       <c r="I52" s="29"/>
-      <c r="J52" s="26"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J52" s="29"/>
+      <c r="K52" s="26"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="23"/>
       <c r="C53" s="24"/>
@@ -1724,9 +1781,10 @@
       <c r="G53" s="24"/>
       <c r="H53" s="25"/>
       <c r="I53" s="29"/>
-      <c r="J53" s="26"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="29"/>
+      <c r="K53" s="26"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="23"/>
       <c r="C54" s="24"/>
@@ -1736,9 +1794,10 @@
       <c r="G54" s="24"/>
       <c r="H54" s="25"/>
       <c r="I54" s="29"/>
-      <c r="J54" s="26"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J54" s="29"/>
+      <c r="K54" s="26"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="23"/>
       <c r="C55" s="24"/>
@@ -1748,9 +1807,10 @@
       <c r="G55" s="24"/>
       <c r="H55" s="25"/>
       <c r="I55" s="29"/>
-      <c r="J55" s="26"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J55" s="29"/>
+      <c r="K55" s="26"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="23"/>
       <c r="C56" s="24"/>
@@ -1760,9 +1820,10 @@
       <c r="G56" s="24"/>
       <c r="H56" s="25"/>
       <c r="I56" s="29"/>
-      <c r="J56" s="26"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="29"/>
+      <c r="K56" s="26"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="23"/>
       <c r="C57" s="24"/>
@@ -1772,9 +1833,10 @@
       <c r="G57" s="24"/>
       <c r="H57" s="25"/>
       <c r="I57" s="29"/>
-      <c r="J57" s="26"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J57" s="29"/>
+      <c r="K57" s="26"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="23"/>
       <c r="C58" s="24"/>
@@ -1784,9 +1846,10 @@
       <c r="G58" s="24"/>
       <c r="H58" s="25"/>
       <c r="I58" s="29"/>
-      <c r="J58" s="26"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J58" s="29"/>
+      <c r="K58" s="26"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="23"/>
       <c r="C59" s="24"/>
@@ -1796,9 +1859,10 @@
       <c r="G59" s="24"/>
       <c r="H59" s="25"/>
       <c r="I59" s="29"/>
-      <c r="J59" s="26"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J59" s="29"/>
+      <c r="K59" s="26"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="23"/>
       <c r="C60" s="24"/>
@@ -1808,9 +1872,10 @@
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
       <c r="I60" s="29"/>
-      <c r="J60" s="26"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J60" s="29"/>
+      <c r="K60" s="26"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="23"/>
       <c r="C61" s="24"/>
@@ -1820,9 +1885,10 @@
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
       <c r="I61" s="29"/>
-      <c r="J61" s="26"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J61" s="29"/>
+      <c r="K61" s="26"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="23"/>
       <c r="C62" s="24"/>
@@ -1832,9 +1898,10 @@
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
       <c r="I62" s="29"/>
-      <c r="J62" s="26"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J62" s="29"/>
+      <c r="K62" s="26"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="23"/>
       <c r="C63" s="24"/>
@@ -1844,9 +1911,10 @@
       <c r="G63" s="24"/>
       <c r="H63" s="25"/>
       <c r="I63" s="29"/>
-      <c r="J63" s="26"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J63" s="29"/>
+      <c r="K63" s="26"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="23"/>
       <c r="C64" s="24"/>
@@ -1856,9 +1924,10 @@
       <c r="G64" s="24"/>
       <c r="H64" s="25"/>
       <c r="I64" s="29"/>
-      <c r="J64" s="26"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J64" s="29"/>
+      <c r="K64" s="26"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="23"/>
       <c r="C65" s="24"/>
@@ -1868,9 +1937,10 @@
       <c r="G65" s="24"/>
       <c r="H65" s="25"/>
       <c r="I65" s="29"/>
-      <c r="J65" s="26"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J65" s="29"/>
+      <c r="K65" s="26"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="23"/>
       <c r="C66" s="24"/>
@@ -1880,9 +1950,10 @@
       <c r="G66" s="24"/>
       <c r="H66" s="25"/>
       <c r="I66" s="29"/>
-      <c r="J66" s="26"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J66" s="29"/>
+      <c r="K66" s="26"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="23"/>
       <c r="C67" s="24"/>
@@ -1892,9 +1963,10 @@
       <c r="G67" s="24"/>
       <c r="H67" s="25"/>
       <c r="I67" s="29"/>
-      <c r="J67" s="26"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J67" s="29"/>
+      <c r="K67" s="26"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="23"/>
       <c r="C68" s="24"/>
@@ -1904,9 +1976,10 @@
       <c r="G68" s="24"/>
       <c r="H68" s="25"/>
       <c r="I68" s="29"/>
-      <c r="J68" s="26"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J68" s="29"/>
+      <c r="K68" s="26"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="23"/>
       <c r="C69" s="24"/>
@@ -1916,9 +1989,10 @@
       <c r="G69" s="24"/>
       <c r="H69" s="25"/>
       <c r="I69" s="29"/>
-      <c r="J69" s="26"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J69" s="29"/>
+      <c r="K69" s="26"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="23"/>
       <c r="C70" s="24"/>
@@ -1928,9 +2002,10 @@
       <c r="G70" s="24"/>
       <c r="H70" s="25"/>
       <c r="I70" s="29"/>
-      <c r="J70" s="26"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J70" s="29"/>
+      <c r="K70" s="26"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="23"/>
       <c r="C71" s="24"/>
@@ -1940,9 +2015,10 @@
       <c r="G71" s="24"/>
       <c r="H71" s="25"/>
       <c r="I71" s="29"/>
-      <c r="J71" s="26"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J71" s="29"/>
+      <c r="K71" s="26"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="23"/>
       <c r="C72" s="30"/>
@@ -1952,9 +2028,10 @@
       <c r="G72" s="24"/>
       <c r="H72" s="25"/>
       <c r="I72" s="29"/>
-      <c r="J72" s="26"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J72" s="29"/>
+      <c r="K72" s="26"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="23"/>
       <c r="C73" s="24"/>
@@ -1964,9 +2041,10 @@
       <c r="G73" s="24"/>
       <c r="H73" s="25"/>
       <c r="I73" s="29"/>
-      <c r="J73" s="26"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J73" s="29"/>
+      <c r="K73" s="26"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="23"/>
       <c r="C74" s="24"/>
@@ -1976,9 +2054,10 @@
       <c r="G74" s="24"/>
       <c r="H74" s="25"/>
       <c r="I74" s="29"/>
-      <c r="J74" s="26"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J74" s="29"/>
+      <c r="K74" s="26"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="23"/>
       <c r="C75" s="24"/>
@@ -1988,20 +2067,21 @@
       <c r="G75" s="24"/>
       <c r="H75" s="25"/>
       <c r="I75" s="29"/>
-      <c r="J75" s="26"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="26"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <autoFilter ref="A2:J75" xr:uid="{52620AD0-D81A-4707-BF25-930520122703}"/>
+  <autoFilter ref="A2:K75" xr:uid="{52620AD0-D81A-4707-BF25-930520122703}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I75" xr:uid="{95136ACE-3B61-4F2E-BC2F-785DA5FB4AA4}">
-      <formula1>$AB$7:$AB$8</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J75" xr:uid="{95136ACE-3B61-4F2E-BC2F-785DA5FB4AA4}">
+      <formula1>$AC$7:$AC$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H75" xr:uid="{A8A29524-CB88-4A40-9BD1-F8E9BD2459CB}">
-      <formula1>$AB$3:$AB$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I75" xr:uid="{A8A29524-CB88-4A40-9BD1-F8E9BD2459CB}">
+      <formula1>$AC$3:$AC$4</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -2043,16 +2123,16 @@
       <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="51" t="s">
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
@@ -2064,60 +2144,60 @@
       <c r="C2" s="14">
         <v>44130</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="42" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="47"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="12"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="47"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="12"/>
       <c r="C4" s="15"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="47"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="12"/>
       <c r="C5" s="15"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="47"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="13"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2135,18 +2215,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>